<commit_message>
pedido produtos custo medio
</commit_message>
<xml_diff>
--- a/meta-2022.xlsx
+++ b/meta-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desenvolvimento\Projetos\Innovation\innovation-etl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE41B0FF-2C69-4580-9C66-AABBEA6C6A0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8D2FDF-CD05-4950-BF80-3CA17629F341}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{7159B005-A463-4E5E-A38D-2CE497116AA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7159B005-A463-4E5E-A38D-2CE497116AA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72C4D2F-2556-47AF-B539-8A3C6A5A0CE9}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,7 +683,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>2500000</v>
       </c>
     </row>
   </sheetData>
@@ -739,7 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13031874-3707-49BF-B583-62B76F7C8EEC}">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A39"/>
     </sheetView>
   </sheetViews>

</xml_diff>